<commit_message>
adding gui for easier use
</commit_message>
<xml_diff>
--- a/HERECON.xlsx
+++ b/HERECON.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,149 +462,130 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7</v>
+      </c>
+      <c r="D2" t="n">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3</v>
-      </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Cheyenne</t>
+          <t>Andrea A</t>
         </is>
       </c>
       <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
         <v>4</v>
-      </c>
-      <c r="C3" t="n">
-        <v>8</v>
-      </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Emir</t>
+          <t>Johana</t>
         </is>
       </c>
       <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>11</v>
+      </c>
+      <c r="D4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Float Board</t>
+          <t>Julio</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Hung Board</t>
+          <t>Mariana</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Johana</t>
+          <t>Nestor</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Mariana</t>
+          <t>Tameka</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Shae</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>5</v>
-      </c>
-      <c r="C9" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed header values to match HE
</commit_message>
<xml_diff>
--- a/HERECON.xlsx
+++ b/HERECON.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,134 +458,172 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Cheyenne</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Andrea A</t>
+          <t>Float Board</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Johana</t>
+          <t>Hung Board</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Julio</t>
+          <t>Johana</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Mariana</t>
+          <t>Juan Carlos</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Nestor</t>
+          <t>Mariana</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Tameka</t>
+          <t>Nestor</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>3</v>
       </c>
       <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
         <v>3</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Shae</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="n">
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Tameka</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
         <v>9</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
will stop saving excel and only display table
</commit_message>
<xml_diff>
--- a/HERECON.xlsx
+++ b/HERECON.xlsx
@@ -436,22 +436,22 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>King Stayover</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>King Checkout</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>King Stayover</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Queen Stayover</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Queen Checkout</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Queen Stayover</t>
         </is>
       </c>
     </row>
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
         <v>11</v>
       </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
       <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>6</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -481,10 +481,10 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
         <v>4</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -506,10 +506,10 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
         <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
         <v>15</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
       <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
         <v>2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
       <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
         <v>7</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -557,16 +557,16 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
         <v>4</v>
       </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
       <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
         <v>11</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -576,16 +576,16 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
         <v>3</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
       <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
         <v>3</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -595,16 +595,16 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
         <v>9</v>
       </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
       <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
         <v>7</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -614,16 +614,16 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="n">
         <v>6</v>
       </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
       <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
         <v>9</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>